<commit_message>
ver7.4 update fixtures excel
</commit_message>
<xml_diff>
--- a/fixtures.xlsx
+++ b/fixtures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1CA4CD-E2B1-427F-8FD3-703D4E76BEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B75902-32C8-4FDC-AB30-E1E8E77D2661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,6 +206,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="172" formatCode="[$-10409]h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -263,13 +267,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -579,7 +583,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:D52"/>
+      <selection activeCell="B2" sqref="B2:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,716 +609,716 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>45619</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>0.85416666666666663</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>45619</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>45619</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>45619</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>45619</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>45619</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>45620</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>45621</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>45622</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>45625</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>45626</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>45627</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>45627</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>45627</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="4">
         <v>0.89583333333333337</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>45628</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>0</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>45629</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>45629</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="4">
         <v>0.17708333333333334</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>45630</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>45630</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>45630</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>45630</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="4">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <v>45630</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>0.17708333333333334</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>45630</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>0.17708333333333334</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>45631</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>0.14583333333333334</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+      <c r="A26" s="3">
         <v>45631</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>0.17708333333333334</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
+      <c r="A27" s="3">
         <v>45633</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>0.85416666666666663</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+      <c r="A28" s="3">
         <v>45633</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
+      <c r="A29" s="3">
         <v>45633</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <v>45633</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <v>45634</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
+      <c r="A32" s="3">
         <v>45634</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
+      <c r="A33" s="3">
         <v>45634</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <v>45634</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
+      <c r="A35" s="3">
         <v>45635</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
+      <c r="A36" s="3">
         <v>45635</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="4">
         <v>0.16666666666666666</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
+      <c r="A37" s="3">
         <v>45640</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
+      <c r="A38" s="3">
         <v>45640</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
+      <c r="A39" s="3">
         <v>45640</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
+      <c r="A40" s="3">
         <v>45640</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
+      <c r="A41" s="3">
         <v>45641</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="4">
         <v>6.25E-2</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
+      <c r="A42" s="3">
         <v>45641</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
+      <c r="A43" s="3">
         <v>45641</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="4">
         <v>0.97916666666666663</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
+      <c r="A44" s="3">
         <v>45642</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
+      <c r="A45" s="3">
         <v>45642</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
+      <c r="A46" s="3">
         <v>45647</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="4">
         <v>0.85416666666666663</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="2">
+      <c r="A47" s="3">
         <v>45647</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
+      <c r="A48" s="3">
         <v>45648</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
+      <c r="A49" s="3">
         <v>45648</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
+      <c r="A50" s="3">
         <v>45648</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="2">
+      <c r="A51" s="3">
         <v>45648</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
+      <c r="A52" s="3">
         <v>45648</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="4">
         <v>0.97916666666666663</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>